<commit_message>
Dedicated Aspose demo was added.
- Added new format templates in order to test Aspose behavior with xlsx (MS and Strict Open Xml).
- Improvement of Excel Viewer, Zoom and pan is now supported.
</commit_message>
<xml_diff>
--- a/AsposeDemo/bin/Debug/templates/Template.xlsx
+++ b/AsposeDemo/bin/Debug/templates/Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jose.mendoza\source\repos\PrintingReport\AsposeDemo\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E27AA768-21D1-4B50-B258-9E2C54E1B3F2}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{163FA65F-4E44-4CCD-A886-94848757C116}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545" xr2:uid="{FCE83E77-3008-498F-B47A-3648F6D66240}"/>
   </bookViews>
@@ -140,16 +140,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -169,118 +169,6 @@
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>438150</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="2" name="txthospitalname">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BFCF8892-2306-48AD-9201-A8158F909969}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="0" y="161925"/>
-          <a:ext cx="1047750" cy="285750"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>66676</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>47626</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="3" name="txtsiteid">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{928C4344-F5AF-4CAB-A42D-A53BF8ECFF38}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="1285876" y="200025"/>
-          <a:ext cx="3638550" cy="247650"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -340,143 +228,6 @@
               <a:latin typeface="Bookman Old Style"/>
             </a:rPr>
             <a:t>ANESTHESIOLOGIST:</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>1076325</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2286000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>85725</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="5" name="txttransactionno">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72B748A2-838F-41D0-9DB3-BEE0F65FD2F7}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="609600" y="1657350"/>
-          <a:ext cx="0" cy="209550"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-US" b="1">
-              <a:latin typeface="Bookman Old Style" pitchFamily="18" charset="0"/>
-            </a:rPr>
-            <a:t>f</a:t>
-          </a:r>
-        </a:p>
-      </xdr:txBody>
-    </xdr:sp>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>133350</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>2752725</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
-    </xdr:to>
-    <xdr:sp macro="" textlink="">
-      <xdr:nvSpPr>
-        <xdr:cNvPr id="6" name="txtlocationidcoded">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{063FAACA-90E9-4D61-8357-6ABD019B39C5}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvSpPr txBox="1">
-          <a:spLocks noChangeArrowheads="1"/>
-        </xdr:cNvSpPr>
-      </xdr:nvSpPr>
-      <xdr:spPr bwMode="auto">
-        <a:xfrm>
-          <a:off x="133350" y="1266825"/>
-          <a:ext cx="476250" cy="361950"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:extLst>
-          <a:ext uri="{91240B29-F687-4F45-9708-019B960494DF}">
-            <a14:hiddenLine xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" w="9525">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:miter lim="800000"/>
-              <a:headEnd/>
-              <a:tailEnd/>
-            </a14:hiddenLine>
-          </a:ext>
-        </a:extLst>
-      </xdr:spPr>
-      <xdr:txBody>
-        <a:bodyPr/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr algn="ctr"/>
-          <a:r>
-            <a:rPr lang="en-US" sz="1800">
-              <a:latin typeface="3 of 9 Barcode" pitchFamily="82" charset="0"/>
-            </a:rPr>
-            <a:t>f</a:t>
           </a:r>
         </a:p>
       </xdr:txBody>
@@ -983,7 +734,7 @@
   <dimension ref="A1:Z94"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+      <selection activeCell="N14" sqref="N14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1471,18 +1222,18 @@
       <c r="Z17" s="1"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A18" s="7"/>
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="8"/>
-      <c r="I18" s="8"/>
-      <c r="J18" s="8"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="8"/>
+      <c r="A18" s="6"/>
+      <c r="B18" s="6"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+      <c r="K18" s="5"/>
+      <c r="L18" s="5"/>
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
@@ -1499,8 +1250,8 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="8"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
@@ -1527,8 +1278,8 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A20" s="5"/>
-      <c r="B20" s="6"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="8"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
@@ -1555,8 +1306,8 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="8"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
@@ -1583,8 +1334,8 @@
       <c r="Z21" s="1"/>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="8"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
@@ -1611,8 +1362,8 @@
       <c r="Z22" s="1"/>
     </row>
     <row r="23" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
-      <c r="B23" s="6"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="8"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
@@ -1639,8 +1390,8 @@
       <c r="Z23" s="1"/>
     </row>
     <row r="24" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A24" s="5"/>
-      <c r="B24" s="6"/>
+      <c r="A24" s="7"/>
+      <c r="B24" s="8"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
@@ -1667,8 +1418,8 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
-      <c r="B25" s="6"/>
+      <c r="A25" s="7"/>
+      <c r="B25" s="8"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
@@ -1695,8 +1446,8 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
+      <c r="A26" s="7"/>
+      <c r="B26" s="8"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
@@ -1723,8 +1474,8 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
-      <c r="B27" s="6"/>
+      <c r="A27" s="7"/>
+      <c r="B27" s="8"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
@@ -1751,8 +1502,8 @@
       <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A28" s="5"/>
-      <c r="B28" s="6"/>
+      <c r="A28" s="7"/>
+      <c r="B28" s="8"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
@@ -1779,8 +1530,8 @@
       <c r="Z28" s="1"/>
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
-      <c r="B29" s="6"/>
+      <c r="A29" s="7"/>
+      <c r="B29" s="8"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
@@ -1807,8 +1558,8 @@
       <c r="Z29" s="1"/>
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A30" s="5"/>
-      <c r="B30" s="6"/>
+      <c r="A30" s="7"/>
+      <c r="B30" s="8"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
@@ -1835,8 +1586,8 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
-      <c r="B31" s="6"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="8"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
       <c r="E31" s="2"/>
@@ -1863,8 +1614,8 @@
       <c r="Z31" s="1"/>
     </row>
     <row r="32" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A32" s="5"/>
-      <c r="B32" s="6"/>
+      <c r="A32" s="7"/>
+      <c r="B32" s="8"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
       <c r="E32" s="2"/>
@@ -1891,8 +1642,8 @@
       <c r="Z32" s="1"/>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
-      <c r="B33" s="6"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="8"/>
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
@@ -1919,8 +1670,8 @@
       <c r="Z33" s="1"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="8"/>
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
@@ -1947,8 +1698,8 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
-      <c r="B35" s="6"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="8"/>
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
@@ -1975,8 +1726,8 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A36" s="5"/>
-      <c r="B36" s="6"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="8"/>
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
@@ -2003,8 +1754,8 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
-      <c r="B37" s="6"/>
+      <c r="A37" s="7"/>
+      <c r="B37" s="8"/>
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
@@ -3628,16 +3379,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:B21"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:B26"/>
-    <mergeCell ref="A27:B27"/>
     <mergeCell ref="A28:B28"/>
     <mergeCell ref="A29:B29"/>
     <mergeCell ref="A36:B36"/>
@@ -3648,6 +3389,16 @@
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A34:B34"/>
     <mergeCell ref="A35:B35"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:B26"/>
+    <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:B21"/>
+    <mergeCell ref="A22:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>